<commit_message>
+ Downsampling and new variable display names
</commit_message>
<xml_diff>
--- a/P10. 2024. Pilot dashboard (1)/Correlation between sensors and stored data.xlsx
+++ b/P10. 2024. Pilot dashboard (1)/Correlation between sensors and stored data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvar\OneDrive - Algiecel ApS\My files\Projects\P10. 2024. Pilot dashboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\Desktop\Speciale\DS_thesis\P10. 2024. Pilot dashboard (1)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1CF7E5-AAE9-4727-BCBA-17C39FD7DB1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B640FE96-6982-418B-97BF-F49043C29719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{86E6F00B-561F-4C9E-8803-61AAA9D61F3F}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{86E6F00B-561F-4C9E-8803-61AAA9D61F3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="83">
   <si>
     <t>Label</t>
   </si>
@@ -259,6 +259,30 @@
   </si>
   <si>
     <t>Did not work for the initial batches</t>
+  </si>
+  <si>
+    <t>fejl</t>
+  </si>
+  <si>
+    <t>Mister top</t>
+  </si>
+  <si>
+    <t>reason:</t>
+  </si>
+  <si>
+    <t>fix efter?</t>
+  </si>
+  <si>
+    <t>Minus</t>
+  </si>
+  <si>
+    <t>binær</t>
+  </si>
+  <si>
+    <t>Binær</t>
+  </si>
+  <si>
+    <t>ens hele vej</t>
   </si>
 </sst>
 </file>
@@ -449,9 +473,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022 Tema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -489,7 +513,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -595,7 +619,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -737,7 +761,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -745,23 +769,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{396551FE-D9F8-4544-82F0-4ACBB58C7B3A}">
-  <dimension ref="C5:I31"/>
+  <dimension ref="A5:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="17.19921875" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" customWidth="1"/>
-    <col min="5" max="6" width="16.46484375" customWidth="1"/>
-    <col min="7" max="7" width="23.59765625" customWidth="1"/>
-    <col min="9" max="9" width="78.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="6" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" customWidth="1"/>
+    <col min="9" max="9" width="78.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="6" spans="3:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="5" t="s">
         <v>0</v>
       </c>
@@ -784,7 +808,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
         <v>4</v>
       </c>
@@ -805,7 +829,7 @@
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
         <v>5</v>
       </c>
@@ -826,7 +850,7 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
         <v>6</v>
       </c>
@@ -847,7 +871,7 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
         <v>10</v>
       </c>
@@ -868,7 +892,7 @@
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
         <v>11</v>
       </c>
@@ -889,7 +913,7 @@
       </c>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
         <v>7</v>
       </c>
@@ -910,7 +934,10 @@
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>77</v>
+      </c>
       <c r="C13" s="2" t="s">
         <v>12</v>
       </c>
@@ -931,7 +958,13 @@
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" t="s">
+        <v>75</v>
+      </c>
       <c r="C14" s="2" t="s">
         <v>13</v>
       </c>
@@ -952,7 +985,13 @@
       </c>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" t="s">
+        <v>76</v>
+      </c>
       <c r="C15" s="2" t="s">
         <v>14</v>
       </c>
@@ -973,7 +1012,7 @@
       </c>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
         <v>8</v>
       </c>
@@ -996,7 +1035,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C17" s="2" t="s">
         <v>15</v>
       </c>
@@ -1017,7 +1056,13 @@
       </c>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" t="s">
+        <v>76</v>
+      </c>
       <c r="C18" s="2" t="s">
         <v>9</v>
       </c>
@@ -1040,7 +1085,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" t="s">
+        <v>75</v>
+      </c>
       <c r="C19" s="2" t="s">
         <v>53</v>
       </c>
@@ -1061,7 +1112,13 @@
       </c>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" t="s">
+        <v>75</v>
+      </c>
       <c r="C20" s="2" t="s">
         <v>54</v>
       </c>
@@ -1082,7 +1139,13 @@
       </c>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" t="s">
+        <v>75</v>
+      </c>
       <c r="C21" s="2" t="s">
         <v>49</v>
       </c>
@@ -1105,7 +1168,13 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>75</v>
+      </c>
       <c r="C22" s="2" t="s">
         <v>16</v>
       </c>
@@ -1126,7 +1195,13 @@
       </c>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>75</v>
+      </c>
       <c r="C23" s="2" t="s">
         <v>17</v>
       </c>
@@ -1147,7 +1222,13 @@
       </c>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>75</v>
+      </c>
       <c r="C24" s="2" t="s">
         <v>18</v>
       </c>
@@ -1168,7 +1249,7 @@
       </c>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C25" s="2" t="s">
         <v>19</v>
       </c>
@@ -1189,7 +1270,7 @@
       </c>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C26" s="2" t="s">
         <v>20</v>
       </c>
@@ -1210,7 +1291,7 @@
       </c>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="3:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="3" t="s">
         <v>21</v>
       </c>
@@ -1231,21 +1312,21 @@
       </c>
       <c r="I27" s="4"/>
     </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C29" s="12" t="s">
         <v>72</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
     </row>
-    <row r="30" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C30" s="13" t="s">
         <v>71</v>
       </c>
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>
     </row>
-    <row r="31" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C31" s="14" t="s">
         <v>70</v>
       </c>

</xml_diff>